<commit_message>
Agent output skeleton, utility of food changed to consider whole meals
Also changed a little bit the .xlsx file to match the fields on the form
</commit_message>
<xml_diff>
--- a/scenarios.xlsx
+++ b/scenarios.xlsx
@@ -1,37 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI_UU\TERM1\IAG\Group project\INFOIAG_project_2021_group1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C5ABAD-5717-43B4-BA2A-48869A5103DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>PreferredCuisine</t>
+  </si>
+  <si>
+    <t>AvoidCuisine</t>
+  </si>
+  <si>
+    <t>PriceRange</t>
+  </si>
+  <si>
+    <t>EatOut</t>
+  </si>
+  <si>
+    <t>Neighbourhood</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>HealthConditions</t>
+  </si>
+  <si>
+    <t>Additional1</t>
+  </si>
+  <si>
+    <t>Additional2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +87,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,220 +414,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Favorite Colour</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>German</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Spanish</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Children</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sven</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="D2" t="b">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="b">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Max</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Tom</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Tokyo</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Marry</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>London</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Jane</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>gggf</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>FYUFYUJY</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3</v>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
form now reads data from owl file
</commit_message>
<xml_diff>
--- a/scenarios.xlsx
+++ b/scenarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>condition_covid</t>
   </si>
@@ -97,6 +97,12 @@
     <t>asdasd</t>
   </si>
   <si>
+    <t>fake food</t>
+  </si>
+  <si>
+    <t>fake food 2</t>
+  </si>
+  <si>
     <t>asdasda</t>
   </si>
   <si>
@@ -115,12 +121,21 @@
     <t>sdaas</t>
   </si>
   <si>
+    <t>real food</t>
+  </si>
+  <si>
+    <t>real food 2</t>
+  </si>
+  <si>
     <t>Moderate</t>
   </si>
   <si>
     <t>Expensive</t>
   </si>
   <si>
+    <t>Cheap</t>
+  </si>
+  <si>
     <t>City 4</t>
   </si>
   <si>
@@ -133,6 +148,12 @@
     <t>City 1</t>
   </si>
   <si>
+    <t>amsterdam</t>
+  </si>
+  <si>
+    <t>innsbruck</t>
+  </si>
+  <si>
     <t>Neighbourhood 2 in City 4</t>
   </si>
   <si>
@@ -143,6 +164,12 @@
   </si>
   <si>
     <t>Neighbourhood 2 in City 1</t>
+  </si>
+  <si>
+    <t>amsterdamNoord</t>
+  </si>
+  <si>
+    <t>reichenau</t>
   </si>
 </sst>
 </file>
@@ -500,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,7 +612,7 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -627,13 +654,13 @@
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="U2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -650,7 +677,7 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -692,13 +719,13 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="T3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="U3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -715,7 +742,7 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -757,13 +784,13 @@
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="T4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="U4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -780,7 +807,7 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -822,13 +849,13 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="T5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="U5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -845,7 +872,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -887,13 +914,13 @@
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="T6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="U6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -910,7 +937,7 @@
         <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -952,13 +979,143 @@
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="U7" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>